<commit_message>
Fix process crash when persion name not in attendance file
</commit_message>
<xml_diff>
--- a/template/考勤彙總報表.xlsx
+++ b/template/考勤彙總報表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="考勤紀錄表 早班" sheetId="1" state="visible" r:id="rId2"/>
@@ -1641,7 +1641,7 @@
   </sheetPr>
   <dimension ref="A1:AH137"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Q8" activeCellId="0" sqref="Q8"/>
@@ -1657,9 +1657,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="0" width="6.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="18" style="0" width="6.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="7.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="24" style="0" width="6.99"/>
   </cols>
@@ -9244,7 +9244,7 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE14" activeCellId="0" sqref="AE14"/>
     </sheetView>
   </sheetViews>
@@ -9255,9 +9255,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="16" style="0" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="18" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="7.88"/>
   </cols>
   <sheetData>

</xml_diff>